<commit_message>
[Add]: DFD muc ngu canh, muc 1
</commit_message>
<xml_diff>
--- a/Báo Cáo/ERD/Đặc tả ERD.xlsx
+++ b/Báo Cáo/ERD/Đặc tả ERD.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Software-Technology\Báo Cáo\ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1663758-4DDD-4EE1-84B8-48D763CC734F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16F0826-F330-4865-A4E9-3B34DA1D2193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34054EE9-184B-4CD0-9EF2-DA9D5A718D52}"/>
   </bookViews>
@@ -1179,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF7D01F-2B17-4ACD-AA2E-CAD07BA1EB35}">
   <dimension ref="A1:Z1059"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166"/>
+    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5305,7 +5305,7 @@
         <v>178</v>
       </c>
       <c r="D122" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E122" s="8"/>
       <c r="F122" s="7"/>
@@ -31798,30 +31798,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B152:F152"/>
     <mergeCell ref="B153:F153"/>
@@ -31838,6 +31814,30 @@
     <mergeCell ref="B103:F103"/>
     <mergeCell ref="B104:F104"/>
     <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Modified]: DFD vi thanh toan
</commit_message>
<xml_diff>
--- a/Báo Cáo/ERD/Đặc tả ERD.xlsx
+++ b/Báo Cáo/ERD/Đặc tả ERD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Software-Technology\Báo Cáo\ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16F0826-F330-4865-A4E9-3B34DA1D2193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4610FDCA-E966-42C2-9063-B49B8B906DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34054EE9-184B-4CD0-9EF2-DA9D5A718D52}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="12360" xr2:uid="{34054EE9-184B-4CD0-9EF2-DA9D5A718D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1179,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF7D01F-2B17-4ACD-AA2E-CAD07BA1EB35}">
   <dimension ref="A1:Z1059"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2045,7 +2045,7 @@
         <v>44</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
@@ -31798,6 +31798,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B143:F143"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B152:F152"/>
     <mergeCell ref="B153:F153"/>
@@ -31814,30 +31838,6 @@
     <mergeCell ref="B103:F103"/>
     <mergeCell ref="B104:F104"/>
     <mergeCell ref="B119:F119"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Modified]: Dac ta ERD
</commit_message>
<xml_diff>
--- a/Báo Cáo/ERD/Đặc tả ERD.xlsx
+++ b/Báo Cáo/ERD/Đặc tả ERD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Software-Technology\Báo Cáo\ERD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4610FDCA-E966-42C2-9063-B49B8B906DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB8DEA1-9EFD-4658-A558-6627632D8DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="23040" windowHeight="12360" xr2:uid="{34054EE9-184B-4CD0-9EF2-DA9D5A718D52}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{34054EE9-184B-4CD0-9EF2-DA9D5A718D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="214">
   <si>
     <t>Field name</t>
   </si>
@@ -674,6 +674,9 @@
   <si>
     <t>text</t>
   </si>
+  <si>
+    <t>Mã chức vụ</t>
+  </si>
 </sst>
 </file>
 
@@ -1177,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FF7D01F-2B17-4ACD-AA2E-CAD07BA1EB35}">
-  <dimension ref="A1:Z1059"/>
+  <dimension ref="A1:Z1060"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A137" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1626,7 +1629,7 @@
         <v>7</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>118</v>
@@ -1664,7 +1667,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>119</v>
@@ -4350,9 +4353,11 @@
         <v>7</v>
       </c>
       <c r="E94" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F94" s="8"/>
+        <v>120</v>
+      </c>
+      <c r="F94" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -5637,20 +5642,16 @@
     <row r="132" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A132" s="4"/>
       <c r="B132" s="6" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="C132" s="7" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="D132" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E132" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="F132" s="7" t="s">
-        <v>181</v>
-      </c>
+      <c r="E132" s="8"/>
+      <c r="F132" s="7"/>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
@@ -5675,10 +5676,10 @@
     <row r="133" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A133" s="4"/>
       <c r="B133" s="6" t="s">
-        <v>157</v>
+        <v>8</v>
       </c>
       <c r="C133" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D133" s="7" t="s">
         <v>10</v>
@@ -5709,10 +5710,10 @@
     <row r="134" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A134" s="4"/>
       <c r="B134" s="6" t="s">
-        <v>8</v>
+        <v>160</v>
       </c>
       <c r="C134" s="7" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D134" s="7" t="s">
         <v>10</v>
@@ -5743,13 +5744,13 @@
     <row r="135" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A135" s="4"/>
       <c r="B135" s="6" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C135" s="7" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D135" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E135" s="8"/>
       <c r="F135" s="7"/>
@@ -5777,13 +5778,13 @@
     <row r="136" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A136" s="4"/>
       <c r="B136" s="6" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C136" s="7" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D136" s="7" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E136" s="8"/>
       <c r="F136" s="7"/>
@@ -5811,10 +5812,10 @@
     <row r="137" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A137" s="4"/>
       <c r="B137" s="6" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C137" s="7" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D137" s="7" t="s">
         <v>10</v>
@@ -5845,10 +5846,10 @@
     <row r="138" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A138" s="4"/>
       <c r="B138" s="6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="C138" s="7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D138" s="7" t="s">
         <v>10</v>
@@ -5879,10 +5880,10 @@
     <row r="139" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A139" s="4"/>
       <c r="B139" s="6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C139" s="7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D139" s="7" t="s">
         <v>10</v>
@@ -5913,16 +5914,16 @@
     <row r="140" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A140" s="4"/>
       <c r="B140" s="6" t="s">
-        <v>169</v>
+        <v>18</v>
       </c>
       <c r="C140" s="7" t="s">
-        <v>170</v>
+        <v>46</v>
       </c>
       <c r="D140" s="7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E140" s="8"/>
-      <c r="F140" s="7"/>
+      <c r="F140" s="8"/>
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
@@ -5946,17 +5947,13 @@
     </row>
     <row r="141" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A141" s="4"/>
-      <c r="B141" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C141" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D141" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E141" s="8"/>
-      <c r="F141" s="8"/>
+      <c r="B141" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="11"/>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
@@ -5981,7 +5978,7 @@
     <row r="142" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A142" s="4"/>
       <c r="B142" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C142" s="10"/>
       <c r="D142" s="10"/>
@@ -6010,13 +6007,19 @@
     </row>
     <row r="143" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A143" s="4"/>
-      <c r="B143" s="9" t="s">
-        <v>188</v>
-      </c>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10"/>
-      <c r="E143" s="10"/>
-      <c r="F143" s="11"/>
+      <c r="B143" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D143" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="F143" s="8"/>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
@@ -6041,18 +6044,18 @@
     <row r="144" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A144" s="4"/>
       <c r="B144" s="6" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
       <c r="C144" s="7" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
       <c r="D144" s="7" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E144" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F144" s="8"/>
+        <v>191</v>
+      </c>
+      <c r="F144" s="7"/>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
@@ -6077,16 +6080,16 @@
     <row r="145" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A145" s="4"/>
       <c r="B145" s="6" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="C145" s="7" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D145" s="7" t="s">
         <v>10</v>
       </c>
       <c r="E145" s="7" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F145" s="7"/>
       <c r="G145" s="2"/>
@@ -6113,17 +6116,15 @@
     <row r="146" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A146" s="4"/>
       <c r="B146" s="6" t="s">
-        <v>192</v>
+        <v>175</v>
       </c>
       <c r="C146" s="7" t="s">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="D146" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E146" s="7" t="s">
-        <v>194</v>
-      </c>
+      <c r="E146" s="7"/>
       <c r="F146" s="7"/>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
@@ -6681,7 +6682,7 @@
       <c r="Z162" s="2"/>
     </row>
     <row r="163" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A163" s="2"/>
+      <c r="A163" s="4"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
@@ -31796,32 +31797,11 @@
       <c r="Y1059" s="2"/>
       <c r="Z1059" s="2"/>
     </row>
+    <row r="1060" spans="1:26" ht="24.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1060" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="B142:F142"/>
-    <mergeCell ref="B143:F143"/>
-    <mergeCell ref="B148:F148"/>
-    <mergeCell ref="B149:F149"/>
-    <mergeCell ref="B120:F120"/>
-    <mergeCell ref="B124:F124"/>
-    <mergeCell ref="B125:F125"/>
-    <mergeCell ref="B128:F128"/>
-    <mergeCell ref="B129:F129"/>
-    <mergeCell ref="B61:F61"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
     <mergeCell ref="B62:F62"/>
     <mergeCell ref="B152:F152"/>
     <mergeCell ref="B153:F153"/>
@@ -31838,6 +31818,30 @@
     <mergeCell ref="B103:F103"/>
     <mergeCell ref="B104:F104"/>
     <mergeCell ref="B119:F119"/>
+    <mergeCell ref="B61:F61"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B50:F50"/>
+    <mergeCell ref="B51:F51"/>
+    <mergeCell ref="B55:F55"/>
+    <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B141:F141"/>
+    <mergeCell ref="B142:F142"/>
+    <mergeCell ref="B148:F148"/>
+    <mergeCell ref="B149:F149"/>
+    <mergeCell ref="B120:F120"/>
+    <mergeCell ref="B124:F124"/>
+    <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B128:F128"/>
+    <mergeCell ref="B129:F129"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>